<commit_message>
Dicionario de dados e MER
</commit_message>
<xml_diff>
--- a/StartIdea/StartIdea.Docs/Dicionário de Dados.xlsx
+++ b/StartIdea/StartIdea.Docs/Dicionário de Dados.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="154">
   <si>
     <t>Atributo</t>
   </si>
@@ -354,15 +354,6 @@
     <t>Data de exclusao do product backlog item</t>
   </si>
   <si>
-    <t>Entidade: InteracaoProductBacklogItem</t>
-  </si>
-  <si>
-    <t>TipoInteracao</t>
-  </si>
-  <si>
-    <t>DataInteracao</t>
-  </si>
-  <si>
     <t>MembroTimeId</t>
   </si>
   <si>
@@ -378,15 +369,6 @@
     <t>Mensagem da interação</t>
   </si>
   <si>
-    <t>Data/Hora da interação</t>
-  </si>
-  <si>
-    <t>Identificador do product backlog item vinculado a interação</t>
-  </si>
-  <si>
-    <t>Identificador do membro do time relacionado a interação</t>
-  </si>
-  <si>
     <t>Entidade:  Reuniao</t>
   </si>
   <si>
@@ -432,9 +414,6 @@
     <t>Descrição: Armazena os dados pertinentes ao time</t>
   </si>
   <si>
-    <t>Descrição: Armazena os dados pertinentes a interação do product backlog item</t>
-  </si>
-  <si>
     <t>Descrição: Armazena os dados pertinentes a tarefa</t>
   </si>
   <si>
@@ -484,6 +463,24 @@
   </si>
   <si>
     <t>Entidade: ProductBacklog</t>
+  </si>
+  <si>
+    <t>Entidade: HistoricoEstimativa</t>
+  </si>
+  <si>
+    <t>ProductBacklogId</t>
+  </si>
+  <si>
+    <t>Descrição: Armazena os dados pertinentes aos históricos das estimativas</t>
+  </si>
+  <si>
+    <t>ProductBacklog</t>
+  </si>
+  <si>
+    <t>Identificador do membro do time responsavel pela estimativa</t>
+  </si>
+  <si>
+    <t>Identificador do product backlog vinculado a estimativa</t>
   </si>
 </sst>
 </file>
@@ -678,6 +675,15 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -707,14 +713,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -729,9 +729,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1076,10 +1073,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F158"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122:F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,52 +1090,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1243,23 +1240,23 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="27"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="4" t="s">
         <v>11</v>
       </c>
@@ -1272,8 +1269,8 @@
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="1" t="s">
@@ -1281,32 +1278,32 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="20"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="23"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
@@ -1399,23 +1396,23 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="23"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="13"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="12"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="4" t="s">
         <v>11</v>
       </c>
@@ -1428,10 +1425,10 @@
       <c r="A25" s="10">
         <v>1</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="14"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="2" t="s">
         <v>20</v>
       </c>
@@ -1444,10 +1441,10 @@
       <c r="A26" s="10">
         <v>2</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="14"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="2" t="s">
         <v>20</v>
       </c>
@@ -1457,24 +1454,24 @@
       <c r="F26" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="17"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="20"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="20"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="23"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -1533,23 +1530,23 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="23"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="13"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="12"/>
+      <c r="C34" s="15"/>
       <c r="D34" s="4" t="s">
         <v>11</v>
       </c>
@@ -1562,10 +1559,10 @@
       <c r="A35" s="10">
         <v>1</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="14"/>
+      <c r="C35" s="17"/>
       <c r="D35" s="2" t="s">
         <v>20</v>
       </c>
@@ -1575,24 +1572,24 @@
       <c r="F35" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="17"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="20"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="20"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="23"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
@@ -1651,23 +1648,23 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="23"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="13"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="12"/>
+      <c r="C43" s="15"/>
       <c r="D43" s="4" t="s">
         <v>11</v>
       </c>
@@ -1680,10 +1677,10 @@
       <c r="A44" s="10">
         <v>1</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="14"/>
+      <c r="C44" s="17"/>
       <c r="D44" s="2" t="s">
         <v>20</v>
       </c>
@@ -1693,24 +1690,24 @@
       <c r="F44" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="17"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="20"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="20"/>
+      <c r="A47" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="23"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
@@ -1785,23 +1782,23 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="21" t="s">
+      <c r="A52" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B52" s="22"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="23"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="13"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C53" s="12"/>
+      <c r="C53" s="15"/>
       <c r="D53" s="4" t="s">
         <v>11</v>
       </c>
@@ -1814,10 +1811,10 @@
       <c r="A54" s="10">
         <v>1</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="14"/>
+      <c r="C54" s="17"/>
       <c r="D54" s="2" t="s">
         <v>20</v>
       </c>
@@ -1827,24 +1824,24 @@
       <c r="F54" s="1"/>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="17"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="20"/>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="18" t="s">
+      <c r="A57" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B57" s="19"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="20"/>
+      <c r="B57" s="22"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="23"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
@@ -1983,23 +1980,23 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="21" t="s">
+      <c r="A66" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B66" s="22"/>
-      <c r="C66" s="22"/>
-      <c r="D66" s="22"/>
-      <c r="E66" s="22"/>
-      <c r="F66" s="23"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="13"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="B67" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C67" s="12"/>
+      <c r="C67" s="15"/>
       <c r="D67" s="4" t="s">
         <v>11</v>
       </c>
@@ -2012,10 +2009,10 @@
       <c r="A68" s="10">
         <v>1</v>
       </c>
-      <c r="B68" s="13" t="s">
+      <c r="B68" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C68" s="14"/>
+      <c r="C68" s="17"/>
       <c r="D68" s="2" t="s">
         <v>20</v>
       </c>
@@ -2025,24 +2022,24 @@
       <c r="F68" s="1"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="16"/>
-      <c r="E70" s="16"/>
-      <c r="F70" s="17"/>
+      <c r="A70" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="20"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="B71" s="19"/>
-      <c r="C71" s="19"/>
-      <c r="D71" s="19"/>
-      <c r="E71" s="19"/>
-      <c r="F71" s="20"/>
+      <c r="A71" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B71" s="22"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="23"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
@@ -2181,23 +2178,23 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="21" t="s">
+      <c r="A80" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B80" s="22"/>
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="23"/>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="13"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B81" s="11" t="s">
+      <c r="B81" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C81" s="12"/>
+      <c r="C81" s="15"/>
       <c r="D81" s="4" t="s">
         <v>11</v>
       </c>
@@ -2210,10 +2207,10 @@
       <c r="A82" s="10">
         <v>1</v>
       </c>
-      <c r="B82" s="13" t="s">
+      <c r="B82" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C82" s="14"/>
+      <c r="C82" s="17"/>
       <c r="D82" s="2" t="s">
         <v>20</v>
       </c>
@@ -2223,24 +2220,24 @@
       <c r="F82" s="1"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="15" t="s">
+      <c r="A84" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B84" s="16"/>
-      <c r="C84" s="16"/>
-      <c r="D84" s="16"/>
-      <c r="E84" s="16"/>
-      <c r="F84" s="17"/>
+      <c r="B84" s="19"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="19"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="20"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="B85" s="19"/>
-      <c r="C85" s="19"/>
-      <c r="D85" s="19"/>
-      <c r="E85" s="19"/>
-      <c r="F85" s="20"/>
+      <c r="A85" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B85" s="22"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="23"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
@@ -2317,23 +2314,23 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="21" t="s">
+      <c r="A90" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B90" s="22"/>
-      <c r="C90" s="22"/>
-      <c r="D90" s="22"/>
-      <c r="E90" s="22"/>
-      <c r="F90" s="23"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="13"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B91" s="11" t="s">
+      <c r="B91" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C91" s="12"/>
+      <c r="C91" s="15"/>
       <c r="D91" s="4" t="s">
         <v>11</v>
       </c>
@@ -2346,10 +2343,10 @@
       <c r="A92" s="10">
         <v>1</v>
       </c>
-      <c r="B92" s="13" t="s">
+      <c r="B92" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C92" s="14"/>
+      <c r="C92" s="17"/>
       <c r="D92" s="2" t="s">
         <v>20</v>
       </c>
@@ -2362,10 +2359,10 @@
       <c r="A93" s="10">
         <v>1</v>
       </c>
-      <c r="B93" s="13" t="s">
+      <c r="B93" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C93" s="14"/>
+      <c r="C93" s="17"/>
       <c r="D93" s="2" t="s">
         <v>20</v>
       </c>
@@ -2375,24 +2372,24 @@
       <c r="F93" s="1"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B95" s="16"/>
-      <c r="C95" s="16"/>
-      <c r="D95" s="16"/>
-      <c r="E95" s="16"/>
-      <c r="F95" s="17"/>
+      <c r="A95" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B95" s="19"/>
+      <c r="C95" s="19"/>
+      <c r="D95" s="19"/>
+      <c r="E95" s="19"/>
+      <c r="F95" s="20"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="B96" s="19"/>
-      <c r="C96" s="19"/>
-      <c r="D96" s="19"/>
-      <c r="E96" s="19"/>
-      <c r="F96" s="20"/>
+      <c r="A96" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B96" s="22"/>
+      <c r="C96" s="22"/>
+      <c r="D96" s="22"/>
+      <c r="E96" s="22"/>
+      <c r="F96" s="23"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
@@ -2531,23 +2528,23 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="21" t="s">
+      <c r="A105" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B105" s="22"/>
-      <c r="C105" s="22"/>
-      <c r="D105" s="22"/>
-      <c r="E105" s="22"/>
-      <c r="F105" s="23"/>
+      <c r="B105" s="12"/>
+      <c r="C105" s="12"/>
+      <c r="D105" s="12"/>
+      <c r="E105" s="12"/>
+      <c r="F105" s="13"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B106" s="11" t="s">
+      <c r="B106" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C106" s="12"/>
+      <c r="C106" s="15"/>
       <c r="D106" s="4" t="s">
         <v>11</v>
       </c>
@@ -2560,10 +2557,10 @@
       <c r="A107" s="10">
         <v>1</v>
       </c>
-      <c r="B107" s="13" t="s">
+      <c r="B107" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C107" s="14"/>
+      <c r="C107" s="17"/>
       <c r="D107" s="2" t="s">
         <v>20</v>
       </c>
@@ -2573,24 +2570,24 @@
       <c r="F107" s="1"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B109" s="16"/>
-      <c r="C109" s="16"/>
-      <c r="D109" s="16"/>
-      <c r="E109" s="16"/>
-      <c r="F109" s="17"/>
+      <c r="A109" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B109" s="19"/>
+      <c r="C109" s="19"/>
+      <c r="D109" s="19"/>
+      <c r="E109" s="19"/>
+      <c r="F109" s="20"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="B110" s="19"/>
-      <c r="C110" s="19"/>
-      <c r="D110" s="19"/>
-      <c r="E110" s="19"/>
-      <c r="F110" s="20"/>
+      <c r="A110" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="B110" s="22"/>
+      <c r="C110" s="22"/>
+      <c r="D110" s="22"/>
+      <c r="E110" s="22"/>
+      <c r="F110" s="23"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
@@ -2627,7 +2624,7 @@
       </c>
       <c r="E112" s="10"/>
       <c r="F112" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -2635,7 +2632,7 @@
         <v>2</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>69</v>
@@ -2643,7 +2640,7 @@
       <c r="D113" s="10"/>
       <c r="E113" s="10"/>
       <c r="F113" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -2651,7 +2648,7 @@
         <v>3</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>60</v>
@@ -2659,7 +2656,7 @@
       <c r="D114" s="10"/>
       <c r="E114" s="10"/>
       <c r="F114" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -2667,15 +2664,17 @@
         <v>4</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>113</v>
+        <v>149</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D115" s="10"/>
-      <c r="E115" s="10"/>
+      <c r="E115" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="F115" s="1" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -2683,7 +2682,7 @@
         <v>5</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>69</v>
@@ -2693,181 +2692,181 @@
         <v>35</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="9">
-        <v>6</v>
-      </c>
-      <c r="B117" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D117" s="10"/>
-      <c r="E117" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>121</v>
-      </c>
+      <c r="A117" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B117" s="12"/>
+      <c r="C117" s="12"/>
+      <c r="D117" s="12"/>
+      <c r="E117" s="12"/>
+      <c r="F117" s="13"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B118" s="22"/>
-      <c r="C118" s="22"/>
-      <c r="D118" s="22"/>
-      <c r="E118" s="22"/>
-      <c r="F118" s="23"/>
+      <c r="A118" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C118" s="15"/>
+      <c r="D118" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E118" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F118" s="4"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B119" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C119" s="12"/>
-      <c r="D119" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E119" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F119" s="4"/>
+      <c r="A119" s="10">
+        <v>1</v>
+      </c>
+      <c r="B119" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C119" s="17"/>
+      <c r="D119" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F119" s="1"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="10">
-        <v>1</v>
-      </c>
-      <c r="B120" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C120" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C120" s="17"/>
       <c r="D120" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="F120" s="1"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="10">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B122" s="19"/>
+      <c r="C122" s="19"/>
+      <c r="D122" s="19"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="20"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B123" s="22"/>
+      <c r="C123" s="22"/>
+      <c r="D123" s="22"/>
+      <c r="E123" s="22"/>
+      <c r="F123" s="23"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F124" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="8">
+        <v>1</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D125" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E125" s="10"/>
+      <c r="F125" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="9">
         <v>2</v>
       </c>
-      <c r="B121" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C121" s="14"/>
-      <c r="D121" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F121" s="1"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B123" s="16"/>
-      <c r="C123" s="16"/>
-      <c r="D123" s="16"/>
-      <c r="E123" s="16"/>
-      <c r="F123" s="17"/>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="B124" s="19"/>
-      <c r="C124" s="19"/>
-      <c r="D124" s="19"/>
-      <c r="E124" s="19"/>
-      <c r="F124" s="20"/>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B125" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C125" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D125" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E125" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F125" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="8">
-        <v>1</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>20</v>
+      <c r="B126" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D126" s="10" t="s">
-        <v>8</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="D126" s="10"/>
       <c r="E126" s="10"/>
       <c r="F126" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
       <c r="D127" s="10"/>
       <c r="E127" s="10"/>
       <c r="F127" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="9">
-        <v>3</v>
-      </c>
-      <c r="B128" s="7" t="s">
-        <v>101</v>
+      <c r="A128" s="8">
+        <v>4</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D128" s="10"/>
-      <c r="E128" s="10"/>
+      <c r="E128" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="F128" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="8">
-        <v>4</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>124</v>
+      <c r="A129" s="9">
+        <v>5</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>69</v>
@@ -2877,165 +2876,165 @@
         <v>35</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="9">
-        <v>5</v>
-      </c>
-      <c r="B130" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D130" s="10"/>
-      <c r="E130" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>130</v>
-      </c>
+      <c r="A130" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B130" s="12"/>
+      <c r="C130" s="12"/>
+      <c r="D130" s="12"/>
+      <c r="E130" s="12"/>
+      <c r="F130" s="13"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B131" s="22"/>
-      <c r="C131" s="22"/>
-      <c r="D131" s="22"/>
-      <c r="E131" s="22"/>
-      <c r="F131" s="23"/>
+      <c r="A131" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B131" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C131" s="15"/>
+      <c r="D131" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E131" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F131" s="4"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B132" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C132" s="12"/>
-      <c r="D132" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E132" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F132" s="4"/>
+      <c r="A132" s="10">
+        <v>1</v>
+      </c>
+      <c r="B132" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C132" s="17"/>
+      <c r="D132" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F132" s="1"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="10">
-        <v>1</v>
-      </c>
-      <c r="B133" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C133" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="B133" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C133" s="17"/>
       <c r="D133" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="F133" s="1"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="10">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B135" s="19"/>
+      <c r="C135" s="19"/>
+      <c r="D135" s="19"/>
+      <c r="E135" s="19"/>
+      <c r="F135" s="20"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="B136" s="22"/>
+      <c r="C136" s="22"/>
+      <c r="D136" s="22"/>
+      <c r="E136" s="22"/>
+      <c r="F136" s="23"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F137" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="8">
+        <v>1</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D138" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E138" s="10"/>
+      <c r="F138" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="9">
         <v>2</v>
       </c>
-      <c r="B134" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C134" s="14"/>
-      <c r="D134" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E134" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F134" s="1"/>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B136" s="16"/>
-      <c r="C136" s="16"/>
-      <c r="D136" s="16"/>
-      <c r="E136" s="16"/>
-      <c r="F136" s="17"/>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B137" s="19"/>
-      <c r="C137" s="19"/>
-      <c r="D137" s="19"/>
-      <c r="E137" s="19"/>
-      <c r="F137" s="20"/>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B138" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C138" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D138" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E138" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F138" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" s="8">
-        <v>1</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>20</v>
+      <c r="B139" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D139" s="10" t="s">
-        <v>8</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D139" s="10"/>
       <c r="E139" s="10"/>
       <c r="F139" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D140" s="10"/>
-      <c r="E140" s="10"/>
+      <c r="E140" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="F140" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A141" s="9">
-        <v>3</v>
-      </c>
-      <c r="B141" s="7" t="s">
-        <v>140</v>
+      <c r="A141" s="8">
+        <v>4</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>69</v>
@@ -3045,15 +3044,15 @@
         <v>35</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" s="8">
-        <v>4</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>141</v>
+      <c r="A142" s="9">
+        <v>5</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>69</v>
@@ -3063,154 +3062,152 @@
         <v>35</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" s="9">
-        <v>5</v>
-      </c>
-      <c r="B143" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D143" s="10"/>
-      <c r="E143" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="A143" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B143" s="12"/>
+      <c r="C143" s="12"/>
+      <c r="D143" s="12"/>
+      <c r="E143" s="12"/>
+      <c r="F143" s="13"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B144" s="22"/>
-      <c r="C144" s="22"/>
-      <c r="D144" s="22"/>
-      <c r="E144" s="22"/>
-      <c r="F144" s="23"/>
+      <c r="A144" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B144" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144" s="15"/>
+      <c r="D144" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E144" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F144" s="4"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B145" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C145" s="12"/>
-      <c r="D145" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E145" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F145" s="4"/>
+      <c r="A145" s="10">
+        <v>1</v>
+      </c>
+      <c r="B145" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C145" s="17"/>
+      <c r="D145" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F145" s="1"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="10">
-        <v>1</v>
-      </c>
-      <c r="B146" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="C146" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="B146" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C146" s="17"/>
       <c r="D146" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F146" s="1"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="10">
-        <v>2</v>
-      </c>
-      <c r="B147" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C147" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="B147" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C147" s="17"/>
       <c r="D147" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
       <c r="F147" s="1"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148" s="10">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B149" s="19"/>
+      <c r="C149" s="19"/>
+      <c r="D149" s="19"/>
+      <c r="E149" s="19"/>
+      <c r="F149" s="20"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B150" s="22"/>
+      <c r="C150" s="22"/>
+      <c r="D150" s="22"/>
+      <c r="E150" s="22"/>
+      <c r="F150" s="23"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C151" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B148" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="C148" s="14"/>
-      <c r="D148" s="2" t="s">
+      <c r="D151" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E151" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F151" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="8">
+        <v>1</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E148" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F148" s="1"/>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="B150" s="16"/>
-      <c r="C150" s="16"/>
-      <c r="D150" s="16"/>
-      <c r="E150" s="16"/>
-      <c r="F150" s="17"/>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="B151" s="19"/>
-      <c r="C151" s="19"/>
-      <c r="D151" s="19"/>
-      <c r="E151" s="19"/>
-      <c r="F151" s="20"/>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B152" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C152" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D152" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E152" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F152" s="4" t="s">
-        <v>1</v>
+      <c r="C152" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D152" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E152" s="10"/>
+      <c r="F152" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A153" s="8">
-        <v>1</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>20</v>
+      <c r="A153" s="9">
+        <v>2</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D153" s="10" t="s">
-        <v>8</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D153" s="10"/>
       <c r="E153" s="10"/>
       <c r="F153" s="1" t="s">
         <v>145</v>
@@ -3218,115 +3215,81 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D154" s="10"/>
       <c r="E154" s="10"/>
       <c r="F154" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A155" s="9">
-        <v>3</v>
-      </c>
-      <c r="B155" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D155" s="10"/>
-      <c r="E155" s="10"/>
-      <c r="F155" s="1" t="s">
-        <v>153</v>
-      </c>
+      <c r="A155" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B155" s="12"/>
+      <c r="C155" s="12"/>
+      <c r="D155" s="12"/>
+      <c r="E155" s="12"/>
+      <c r="F155" s="13"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A156" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B156" s="22"/>
-      <c r="C156" s="22"/>
-      <c r="D156" s="22"/>
-      <c r="E156" s="22"/>
-      <c r="F156" s="23"/>
+      <c r="A156" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B156" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C156" s="15"/>
+      <c r="D156" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E156" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F156" s="4"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A157" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B157" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C157" s="12"/>
-      <c r="D157" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E157" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F157" s="4"/>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A158" s="10" t="s">
+      <c r="A157" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B158" s="13"/>
-      <c r="C158" s="14"/>
-      <c r="D158" s="2"/>
-      <c r="E158" s="2"/>
-      <c r="F158" s="1"/>
+      <c r="B157" s="16"/>
+      <c r="C157" s="17"/>
+      <c r="D157" s="2"/>
+      <c r="E157" s="2"/>
+      <c r="F157" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="A156:F156"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B158:C158"/>
-    <mergeCell ref="B146:C146"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="A150:F150"/>
-    <mergeCell ref="A151:F151"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="A136:F136"/>
-    <mergeCell ref="A137:F137"/>
-    <mergeCell ref="A144:F144"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="A123:F123"/>
-    <mergeCell ref="A124:F124"/>
-    <mergeCell ref="A131:F131"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="B133:C133"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="A71:F71"/>
-    <mergeCell ref="A80:F80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="A56:F56"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A66:F66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="A109:F109"/>
+    <mergeCell ref="A110:F110"/>
+    <mergeCell ref="A117:F117"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="A95:F95"/>
+    <mergeCell ref="A96:F96"/>
+    <mergeCell ref="A105:F105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="A84:F84"/>
+    <mergeCell ref="A85:F85"/>
+    <mergeCell ref="A90:F90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
     <mergeCell ref="A29:F29"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
@@ -3338,29 +3301,47 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A84:F84"/>
-    <mergeCell ref="A85:F85"/>
-    <mergeCell ref="A90:F90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="A95:F95"/>
-    <mergeCell ref="A96:F96"/>
-    <mergeCell ref="A105:F105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="A109:F109"/>
-    <mergeCell ref="A110:F110"/>
-    <mergeCell ref="A118:F118"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A56:F56"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="A71:F71"/>
+    <mergeCell ref="A80:F80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="A122:F122"/>
+    <mergeCell ref="A123:F123"/>
+    <mergeCell ref="A130:F130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="A135:F135"/>
+    <mergeCell ref="A136:F136"/>
+    <mergeCell ref="A143:F143"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B146:C146"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="A149:F149"/>
+    <mergeCell ref="A150:F150"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="1.1811023622047245" right="0.78740157480314965" top="1.1811023622047245" bottom="0.78740157480314965" header="0" footer="0"/>

</xml_diff>